<commit_message>
Ajustes al XLS Reader
</commit_message>
<xml_diff>
--- a/src/test/java/helpers/IHR_Data.xlsx
+++ b/src/test/java/helpers/IHR_Data.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F662E8-75EF-4777-AF0B-E67FBC9CFCB0}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D4F5B3-C549-4DEE-AE7A-A4530A723C0E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Assignee" sheetId="1" r:id="rId1"/>
-    <sheet name="Assignment" sheetId="2" r:id="rId2"/>
+    <sheet name="Assignee" sheetId="2" r:id="rId1"/>
+    <sheet name="AAPolicy" sheetId="1" r:id="rId2"/>
     <sheet name="Policy" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
   <si>
     <t>Australia</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Birth_Date</t>
   </si>
   <si>
-    <t>Mateo</t>
-  </si>
-  <si>
     <t>Ferreira</t>
   </si>
   <si>
@@ -123,22 +120,19 @@
     <t>Home_Country</t>
   </si>
   <si>
-    <t>12/31/1983</t>
-  </si>
-  <si>
-    <t>1/1/2017</t>
-  </si>
-  <si>
-    <t>1/1/2018</t>
-  </si>
-  <si>
-    <t>17032018J</t>
-  </si>
-  <si>
-    <t>722891K</t>
-  </si>
-  <si>
-    <t>924731L</t>
+    <t>Valentina</t>
+  </si>
+  <si>
+    <t>72289739</t>
+  </si>
+  <si>
+    <t>110218</t>
+  </si>
+  <si>
+    <t>1918910605</t>
+  </si>
+  <si>
+    <t>Federico</t>
   </si>
 </sst>
 </file>
@@ -197,13 +191,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -484,11 +477,83 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7271BCF2-BE7D-432D-8482-D32AB698340F}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>42736</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="2">
+        <v>38919</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,7 +562,7 @@
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
@@ -536,49 +601,49 @@
         <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="R1" s="4" t="s">
-        <v>21</v>
-      </c>
       <c r="S1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -586,152 +651,65 @@
         <v>43101</v>
       </c>
       <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>33</v>
+      <c r="D2" s="5">
+        <v>3684367</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="2">
+        <v>37888</v>
       </c>
       <c r="G2" t="s">
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I2" t="s">
         <v>0</v>
       </c>
       <c r="J2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" s="5">
+        <v>447675</v>
+      </c>
+      <c r="L2" s="2">
+        <v>43101</v>
+      </c>
+      <c r="M2" s="2">
+        <v>43646</v>
+      </c>
+      <c r="N2" s="2">
+        <v>43101</v>
+      </c>
+      <c r="O2" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>23</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>24</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>25</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>26</v>
       </c>
-      <c r="S2" t="s">
-        <v>27</v>
-      </c>
-      <c r="T2" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="U2" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7271BCF2-BE7D-432D-8482-D32AB698340F}">
-  <dimension ref="A1:J3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:J2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2">
-        <v>924731</v>
-      </c>
-      <c r="D2" s="2">
+      <c r="T2" s="2">
         <v>43101</v>
       </c>
-      <c r="E2" s="2">
-        <v>43465</v>
-      </c>
-      <c r="F2" s="2">
-        <v>43101</v>
-      </c>
-      <c r="G2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E3" s="3"/>
+      <c r="U2" s="2">
+        <v>37986</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -755,24 +733,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="3">
         <v>43101</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Creacion de policies a traves de Data Driven
</commit_message>
<xml_diff>
--- a/src/test/java/helpers/IHR_Data.xlsx
+++ b/src/test/java/helpers/IHR_Data.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Assignee" sheetId="2" r:id="rId1"/>
     <sheet name="AA" sheetId="3" r:id="rId2"/>
     <sheet name="AAPolicy" sheetId="1" r:id="rId3"/>
+    <sheet name="Policy" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="858" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1003" uniqueCount="359">
   <si>
     <t>Australia</t>
   </si>
@@ -996,6 +997,108 @@
   </si>
   <si>
     <t>XYZ|</t>
+  </si>
+  <si>
+    <t>Policy_Currency</t>
+  </si>
+  <si>
+    <t>Covars_Number</t>
+  </si>
+  <si>
+    <t>Covar1</t>
+  </si>
+  <si>
+    <t>Covar2</t>
+  </si>
+  <si>
+    <t>Covar3</t>
+  </si>
+  <si>
+    <t>Covar4</t>
+  </si>
+  <si>
+    <t>Covar5</t>
+  </si>
+  <si>
+    <t>Covar6</t>
+  </si>
+  <si>
+    <t>Covar7</t>
+  </si>
+  <si>
+    <t>Covar8</t>
+  </si>
+  <si>
+    <t>Covar9</t>
+  </si>
+  <si>
+    <t>Covar10</t>
+  </si>
+  <si>
+    <t>United States Dollar</t>
+  </si>
+  <si>
+    <t>12/31/2018</t>
+  </si>
+  <si>
+    <t>Net Pay</t>
+  </si>
+  <si>
+    <t>zzzAlimony Received</t>
+  </si>
+  <si>
+    <t>zzzAnnual Paid Premium</t>
+  </si>
+  <si>
+    <t>zzzAnnuities</t>
+  </si>
+  <si>
+    <t>zzzAuto Loan Advance</t>
+  </si>
+  <si>
+    <t>zzzAutomobile Expense</t>
+  </si>
+  <si>
+    <t>zzzBase Salary</t>
+  </si>
+  <si>
+    <t>zzzBonus - Current Year</t>
+  </si>
+  <si>
+    <t>zzzEducation Trip</t>
+  </si>
+  <si>
+    <t>zzzEntertainment Allowance</t>
+  </si>
+  <si>
+    <t>Automated Policy28</t>
+  </si>
+  <si>
+    <t>Automated Policy29</t>
+  </si>
+  <si>
+    <t>Automated Policy30</t>
+  </si>
+  <si>
+    <t>Automated Policy31</t>
+  </si>
+  <si>
+    <t>Automated Policy32</t>
+  </si>
+  <si>
+    <t>Automated Policy33</t>
+  </si>
+  <si>
+    <t>Automated Policy34</t>
+  </si>
+  <si>
+    <t>Automated Policy35</t>
+  </si>
+  <si>
+    <t>Automated Policy36</t>
+  </si>
+  <si>
+    <t>Automated Policy37</t>
   </si>
 </sst>
 </file>
@@ -1054,12 +1157,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1887,8 +1991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5300,4 +5404,552 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>349</v>
+      </c>
+      <c r="B2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" s="5">
+        <v>43101</v>
+      </c>
+      <c r="D2" t="s">
+        <v>338</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>339</v>
+      </c>
+      <c r="G2" t="s">
+        <v>340</v>
+      </c>
+      <c r="H2" t="s">
+        <v>341</v>
+      </c>
+      <c r="I2" t="s">
+        <v>342</v>
+      </c>
+      <c r="J2" t="s">
+        <v>343</v>
+      </c>
+      <c r="K2" t="s">
+        <v>344</v>
+      </c>
+      <c r="L2" t="s">
+        <v>345</v>
+      </c>
+      <c r="M2" t="s">
+        <v>346</v>
+      </c>
+      <c r="N2" t="s">
+        <v>347</v>
+      </c>
+      <c r="O2" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>350</v>
+      </c>
+      <c r="B3" t="s">
+        <v>337</v>
+      </c>
+      <c r="C3" s="5">
+        <v>43101</v>
+      </c>
+      <c r="D3" t="s">
+        <v>338</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>339</v>
+      </c>
+      <c r="G3" t="s">
+        <v>340</v>
+      </c>
+      <c r="H3" t="s">
+        <v>341</v>
+      </c>
+      <c r="I3" t="s">
+        <v>342</v>
+      </c>
+      <c r="J3" t="s">
+        <v>343</v>
+      </c>
+      <c r="K3" t="s">
+        <v>344</v>
+      </c>
+      <c r="L3" t="s">
+        <v>345</v>
+      </c>
+      <c r="M3" t="s">
+        <v>346</v>
+      </c>
+      <c r="N3" t="s">
+        <v>347</v>
+      </c>
+      <c r="O3" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>351</v>
+      </c>
+      <c r="B4" t="s">
+        <v>337</v>
+      </c>
+      <c r="C4" s="5">
+        <v>43101</v>
+      </c>
+      <c r="D4" t="s">
+        <v>338</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>339</v>
+      </c>
+      <c r="G4" t="s">
+        <v>340</v>
+      </c>
+      <c r="H4" t="s">
+        <v>341</v>
+      </c>
+      <c r="I4" t="s">
+        <v>342</v>
+      </c>
+      <c r="J4" t="s">
+        <v>343</v>
+      </c>
+      <c r="K4" t="s">
+        <v>344</v>
+      </c>
+      <c r="L4" t="s">
+        <v>345</v>
+      </c>
+      <c r="M4" t="s">
+        <v>346</v>
+      </c>
+      <c r="N4" t="s">
+        <v>347</v>
+      </c>
+      <c r="O4" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>352</v>
+      </c>
+      <c r="B5" t="s">
+        <v>337</v>
+      </c>
+      <c r="C5" s="5">
+        <v>43101</v>
+      </c>
+      <c r="D5" t="s">
+        <v>338</v>
+      </c>
+      <c r="E5">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>339</v>
+      </c>
+      <c r="G5" t="s">
+        <v>340</v>
+      </c>
+      <c r="H5" t="s">
+        <v>341</v>
+      </c>
+      <c r="I5" t="s">
+        <v>342</v>
+      </c>
+      <c r="J5" t="s">
+        <v>343</v>
+      </c>
+      <c r="K5" t="s">
+        <v>344</v>
+      </c>
+      <c r="L5" t="s">
+        <v>345</v>
+      </c>
+      <c r="M5" t="s">
+        <v>346</v>
+      </c>
+      <c r="N5" t="s">
+        <v>347</v>
+      </c>
+      <c r="O5" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>353</v>
+      </c>
+      <c r="B6" t="s">
+        <v>337</v>
+      </c>
+      <c r="C6" s="5">
+        <v>43101</v>
+      </c>
+      <c r="D6" t="s">
+        <v>338</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>339</v>
+      </c>
+      <c r="G6" t="s">
+        <v>340</v>
+      </c>
+      <c r="H6" t="s">
+        <v>341</v>
+      </c>
+      <c r="I6" t="s">
+        <v>342</v>
+      </c>
+      <c r="J6" t="s">
+        <v>343</v>
+      </c>
+      <c r="K6" t="s">
+        <v>344</v>
+      </c>
+      <c r="L6" t="s">
+        <v>345</v>
+      </c>
+      <c r="M6" t="s">
+        <v>346</v>
+      </c>
+      <c r="N6" t="s">
+        <v>347</v>
+      </c>
+      <c r="O6" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>354</v>
+      </c>
+      <c r="B7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C7" s="5">
+        <v>43101</v>
+      </c>
+      <c r="D7" t="s">
+        <v>338</v>
+      </c>
+      <c r="E7">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
+        <v>339</v>
+      </c>
+      <c r="G7" t="s">
+        <v>340</v>
+      </c>
+      <c r="H7" t="s">
+        <v>341</v>
+      </c>
+      <c r="I7" t="s">
+        <v>342</v>
+      </c>
+      <c r="J7" t="s">
+        <v>343</v>
+      </c>
+      <c r="K7" t="s">
+        <v>344</v>
+      </c>
+      <c r="L7" t="s">
+        <v>345</v>
+      </c>
+      <c r="M7" t="s">
+        <v>346</v>
+      </c>
+      <c r="N7" t="s">
+        <v>347</v>
+      </c>
+      <c r="O7" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>355</v>
+      </c>
+      <c r="B8" t="s">
+        <v>337</v>
+      </c>
+      <c r="C8" s="5">
+        <v>43101</v>
+      </c>
+      <c r="D8" t="s">
+        <v>338</v>
+      </c>
+      <c r="E8">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
+        <v>339</v>
+      </c>
+      <c r="G8" t="s">
+        <v>340</v>
+      </c>
+      <c r="H8" t="s">
+        <v>341</v>
+      </c>
+      <c r="I8" t="s">
+        <v>342</v>
+      </c>
+      <c r="J8" t="s">
+        <v>343</v>
+      </c>
+      <c r="K8" t="s">
+        <v>344</v>
+      </c>
+      <c r="L8" t="s">
+        <v>345</v>
+      </c>
+      <c r="M8" t="s">
+        <v>346</v>
+      </c>
+      <c r="N8" t="s">
+        <v>347</v>
+      </c>
+      <c r="O8" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>356</v>
+      </c>
+      <c r="B9" t="s">
+        <v>337</v>
+      </c>
+      <c r="C9" s="5">
+        <v>43101</v>
+      </c>
+      <c r="D9" t="s">
+        <v>338</v>
+      </c>
+      <c r="E9">
+        <v>10</v>
+      </c>
+      <c r="F9" t="s">
+        <v>339</v>
+      </c>
+      <c r="G9" t="s">
+        <v>340</v>
+      </c>
+      <c r="H9" t="s">
+        <v>341</v>
+      </c>
+      <c r="I9" t="s">
+        <v>342</v>
+      </c>
+      <c r="J9" t="s">
+        <v>343</v>
+      </c>
+      <c r="K9" t="s">
+        <v>344</v>
+      </c>
+      <c r="L9" t="s">
+        <v>345</v>
+      </c>
+      <c r="M9" t="s">
+        <v>346</v>
+      </c>
+      <c r="N9" t="s">
+        <v>347</v>
+      </c>
+      <c r="O9" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>357</v>
+      </c>
+      <c r="B10" t="s">
+        <v>337</v>
+      </c>
+      <c r="C10" s="5">
+        <v>43101</v>
+      </c>
+      <c r="D10" t="s">
+        <v>338</v>
+      </c>
+      <c r="E10">
+        <v>10</v>
+      </c>
+      <c r="F10" t="s">
+        <v>339</v>
+      </c>
+      <c r="G10" t="s">
+        <v>340</v>
+      </c>
+      <c r="H10" t="s">
+        <v>341</v>
+      </c>
+      <c r="I10" t="s">
+        <v>342</v>
+      </c>
+      <c r="J10" t="s">
+        <v>343</v>
+      </c>
+      <c r="K10" t="s">
+        <v>344</v>
+      </c>
+      <c r="L10" t="s">
+        <v>345</v>
+      </c>
+      <c r="M10" t="s">
+        <v>346</v>
+      </c>
+      <c r="N10" t="s">
+        <v>347</v>
+      </c>
+      <c r="O10" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>358</v>
+      </c>
+      <c r="B11" t="s">
+        <v>337</v>
+      </c>
+      <c r="C11" s="5">
+        <v>43101</v>
+      </c>
+      <c r="D11" t="s">
+        <v>338</v>
+      </c>
+      <c r="E11">
+        <v>10</v>
+      </c>
+      <c r="F11" t="s">
+        <v>339</v>
+      </c>
+      <c r="G11" t="s">
+        <v>340</v>
+      </c>
+      <c r="H11" t="s">
+        <v>341</v>
+      </c>
+      <c r="I11" t="s">
+        <v>342</v>
+      </c>
+      <c r="J11" t="s">
+        <v>343</v>
+      </c>
+      <c r="K11" t="s">
+        <v>344</v>
+      </c>
+      <c r="L11" t="s">
+        <v>345</v>
+      </c>
+      <c r="M11" t="s">
+        <v>346</v>
+      </c>
+      <c r="N11" t="s">
+        <v>347</v>
+      </c>
+      <c r="O11" t="s">
+        <v>348</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Pay Policy Template Creation
</commit_message>
<xml_diff>
--- a/src/test/java/helpers/IHR_Data.xlsx
+++ b/src/test/java/helpers/IHR_Data.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D73AC67-89C4-48F0-B49B-26F75C3A933E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Assignee" sheetId="2" r:id="rId1"/>
@@ -13,6 +12,7 @@
     <sheet name="AAPolicy" sheetId="1" r:id="rId3"/>
     <sheet name="Policy" sheetId="4" r:id="rId4"/>
     <sheet name="CompImportLegacy" sheetId="5" r:id="rId5"/>
+    <sheet name="NewCompImport" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1011" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1017" uniqueCount="371">
   <si>
     <t>Australia</t>
   </si>
@@ -1125,12 +1125,24 @@
   </si>
   <si>
     <t>C:/Users/mamanrique/Desktop/Test3.xlsx</t>
+  </si>
+  <si>
+    <t>Not Grouping</t>
+  </si>
+  <si>
+    <t>Grouping</t>
+  </si>
+  <si>
+    <t>C:/Users/mamanrique/Desktop/NewCompImportAutomated.xlsx</t>
+  </si>
+  <si>
+    <t>C:/Users/mamanrique/Desktop/NewCompImportAutomated_Grouping.xlsx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
   </numFmts>
@@ -1469,14 +1481,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.85546875" bestFit="1" customWidth="1"/>
@@ -1541,14 +1553,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.28515625" bestFit="1" customWidth="1"/>
@@ -2014,14 +2026,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U52"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="E1" sqref="E1:H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
@@ -5433,14 +5445,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
@@ -5981,14 +5993,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC890CA6-7851-4067-9CF2-79B14B686FAD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="38" bestFit="1" customWidth="1"/>
   </cols>
@@ -6028,4 +6040,46 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="39.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>367</v>
+      </c>
+      <c r="B2" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>368</v>
+      </c>
+      <c r="B3" t="s">
+        <v>370</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>